<commit_message>
Modify Template, add Phoenix contact footprints and 3D models, fix wrong Epson oscillator footprint
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -2,15 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox\Git\KiCAD\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2C28BC-80B5-4CE0-835B-339373D04B41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62929206-FF71-477A-8967-D224DFBC9F1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stückliste" sheetId="1" r:id="rId1"/>
@@ -39,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>Nicht bestückt</t>
   </si>
@@ -1598,8 +1593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="14.25"/>
@@ -1640,7 +1635,7 @@
       <c r="G2" s="89"/>
       <c r="H2" s="87">
         <f ca="1">TODAY()</f>
-        <v>43965</v>
+        <v>43980</v>
       </c>
       <c r="I2" s="87"/>
     </row>
@@ -2148,11 +2143,6 @@
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.59055118110236227" header="0" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="75" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"DINPro,Standard"&amp;9&amp;G&amp;10
-&amp;9&amp;P  / &amp;N</oddFooter>
-  </headerFooter>
-  <legacyDrawingHF r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2160,8 +2150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76DF6D2B-30D7-404F-B8C6-DDD9B17B9EF1}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="14.25"/>
@@ -2185,8 +2175,9 @@
       <c r="F1" s="58"/>
     </row>
     <row r="2" spans="1:6" s="24" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A2" s="89" t="s">
-        <v>43</v>
+      <c r="A2" s="89" t="str">
+        <f>Stückliste!A2</f>
+        <v xml:space="preserve">Bezeichnung / Name: </v>
       </c>
       <c r="B2" s="89"/>
       <c r="C2" s="89"/>
@@ -2194,7 +2185,7 @@
       <c r="E2" s="89"/>
       <c r="F2" s="64">
         <f ca="1">TODAY()</f>
-        <v>43965</v>
+        <v>43980</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="24" customFormat="1" ht="19.899999999999999" customHeight="1">
@@ -2531,11 +2522,6 @@
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.59055118110236227" header="0" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="75" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"DINPro,Standard"&amp;9&amp;G&amp;10
-&amp;9&amp;P  / &amp;N</oddFooter>
-  </headerFooter>
-  <legacyDrawingHF r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2572,7 +2558,7 @@
       <c r="C2" s="39"/>
       <c r="D2" s="34">
         <f ca="1">Stückliste!H2</f>
-        <v>43965</v>
+        <v>43980</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="23" customFormat="1" ht="19.899999999999999" customHeight="1">
@@ -2884,11 +2870,6 @@
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.59055118110236227" header="0" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="75" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"DINPro,Standard"&amp;9&amp;G&amp;10
-&amp;9&amp;P  / &amp;N</oddFooter>
-  </headerFooter>
-  <legacyDrawingHF r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2927,7 +2908,7 @@
       <c r="D2" s="89"/>
       <c r="E2" s="34">
         <f ca="1">Stückliste!H2</f>
-        <v>43965</v>
+        <v>43980</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="19.899999999999999" customHeight="1">
@@ -7602,10 +7583,5 @@
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.59055118110236227" header="0" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="75" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"DINPro,Standard"&amp;9&amp;G&amp;10
-&amp;9&amp;P  / &amp;N</oddFooter>
-  </headerFooter>
-  <legacyDrawingHF r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>